<commit_message>
Auto-committed on 2022/05/09 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L5-管理性作業/HlThreeDetail.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L5-管理性作業/HlThreeDetail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L5-管理性作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC67792D-4308-485C-9157-030BEA9E563F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFDC934-E71A-4628-85EF-1AA6E3EAF3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="115">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -286,10 +286,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>統一編號</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>員工姓名</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -432,14 +428,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>統一編號(單位主管)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>員工姓名(單位主管)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>ActAmt</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -464,7 +452,35 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>OK</t>
+    <t>CdEmp.AgLevel='E'</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdEmp.AgLevel='H'</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>統一編號(單位主管/處長)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>統一編號(主任)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>統一編號(組長)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdEmp.AgLevel='K'</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>統一編號(展業代表)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdEmp.AgLevel='Z'</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -1139,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="17"/>
@@ -1163,12 +1179,12 @@
         <v>19</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="5"/>
       <c r="G1" s="34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1190,7 +1206,7 @@
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>18</v>
@@ -1271,13 +1287,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="26">
         <v>4</v>
@@ -1290,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" s="26">
         <v>7</v>
@@ -1310,13 +1326,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="24">
         <v>3</v>
@@ -1328,13 +1344,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" s="24">
         <v>14</v>
@@ -1348,13 +1364,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="24">
         <v>1</v>
@@ -1367,13 +1383,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="24">
         <v>1</v>
@@ -1389,10 +1405,10 @@
         <v>25</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="24">
         <v>30</v>
@@ -1407,10 +1423,10 @@
         <v>26</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="31">
         <v>6</v>
@@ -1425,10 +1441,10 @@
         <v>20</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="24">
         <v>10</v>
@@ -1442,13 +1458,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="24">
         <v>15</v>
@@ -1462,13 +1478,13 @@
         <v>11</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="24">
         <v>6</v>
@@ -1482,13 +1498,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>54</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="24">
         <v>50</v>
@@ -1502,13 +1518,13 @@
         <v>13</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="24">
         <v>6</v>
@@ -1522,13 +1538,13 @@
         <v>14</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="24">
         <v>20</v>
@@ -1542,13 +1558,13 @@
         <v>15</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>57</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" s="24">
         <v>20</v>
@@ -1568,7 +1584,7 @@
         <v>58</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" s="24">
         <v>20</v>
@@ -1586,7 +1602,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="24">
         <v>8</v>
@@ -1604,7 +1620,7 @@
         <v>60</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" s="24">
         <v>2</v>
@@ -1622,7 +1638,7 @@
         <v>61</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E27" s="24">
         <v>14</v>
@@ -1642,7 +1658,7 @@
         <v>62</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E28" s="24">
         <v>14</v>
@@ -1662,7 +1678,7 @@
         <v>63</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E29" s="24">
         <v>14</v>
@@ -1682,7 +1698,7 @@
         <v>64</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E30" s="24">
         <v>14</v>
@@ -1699,17 +1715,17 @@
         <v>34</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E31" s="24">
         <v>10</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1720,18 +1736,16 @@
         <v>35</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" s="24">
         <v>15</v>
       </c>
       <c r="F32" s="24"/>
-      <c r="G32" s="35" t="s">
-        <v>110</v>
-      </c>
+      <c r="G32" s="35"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="22">
@@ -1741,16 +1755,18 @@
         <v>36</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E33" s="24">
         <v>10</v>
       </c>
       <c r="F33" s="24"/>
-      <c r="G33" s="35"/>
+      <c r="G33" s="35" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="22">
@@ -1763,7 +1779,7 @@
         <v>52</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34" s="24">
         <v>15</v>
@@ -1779,17 +1795,17 @@
         <v>37</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" s="24">
         <v>10</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="35" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1800,18 +1816,16 @@
         <v>22</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="24">
         <v>15</v>
       </c>
       <c r="F36" s="24"/>
-      <c r="G36" s="35" t="s">
-        <v>109</v>
-      </c>
+      <c r="G36" s="35"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="22">
@@ -1821,16 +1835,18 @@
         <v>24</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" s="24">
         <v>10</v>
       </c>
       <c r="F37" s="24"/>
-      <c r="G37" s="35"/>
+      <c r="G37" s="35" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="22">
@@ -1840,10 +1856,10 @@
         <v>23</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="24">
         <v>15</v>
@@ -1862,14 +1878,14 @@
         <v>51</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E39" s="24">
         <v>10</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1880,17 +1896,17 @@
         <v>39</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E40" s="24">
         <v>15</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1901,10 +1917,10 @@
         <v>40</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41" s="24">
         <v>7</v>
@@ -1916,13 +1932,13 @@
         <v>34</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E42" s="24">
         <v>8</v>
@@ -1937,10 +1953,10 @@
         <v>41</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E43" s="24">
         <v>8</v>
@@ -1955,10 +1971,10 @@
         <v>42</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E44" s="24">
         <v>6</v>
@@ -1973,10 +1989,10 @@
         <v>43</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E45" s="24">
         <v>8</v>
@@ -1991,10 +2007,10 @@
         <v>44</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E46" s="24">
         <v>6</v>
@@ -2020,7 +2036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>

</xml_diff>